<commit_message>
Adding percentage data to Lab 10
</commit_message>
<xml_diff>
--- a/10_renal_artery_stenosis/renal_artery_stenosis_data.xlsx
+++ b/10_renal_artery_stenosis/renal_artery_stenosis_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -76,18 +76,6 @@
   </si>
   <si>
     <t>mEq/min</t>
-  </si>
-  <si>
-    <t>PRA(nG aI/mL)/hr</t>
-  </si>
-  <si>
-    <t>Sympathetics (Hz)</t>
-  </si>
-  <si>
-    <t>(L)</t>
-  </si>
-  <si>
-    <t>(mEq/Min)</t>
   </si>
   <si>
     <t>QCP</t>
@@ -103,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +104,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -132,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,63 +157,16 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -230,28 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -259,11 +186,82 @@
       <alignment horizontal="left" indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -553,19 +551,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
@@ -586,12 +586,48 @@
       <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="4"/>
+      <c r="I1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1</v>
+      </c>
+      <c r="W1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A2" s="9"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -608,26 +644,41 @@
         <v>5</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="I2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="5">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30.75" thickBot="1">
+      <c r="I2" s="12"/>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="30.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -649,24 +700,52 @@
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="45.75" thickBot="1">
+      <c r="I3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="4">
+        <v>96.6</v>
+      </c>
+      <c r="K3" s="4">
+        <v>98.8</v>
+      </c>
+      <c r="L3" s="4">
+        <v>100.3</v>
+      </c>
+      <c r="M3" s="4">
+        <v>106.3</v>
+      </c>
+      <c r="N3" s="4">
+        <v>104</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="13">
+        <f>ABS((B3-J3)/B3)</f>
+        <v>4.1237113402062438E-3</v>
+      </c>
+      <c r="T3" s="13">
+        <f t="shared" ref="T3:T9" si="0">ABS((C3-K3)/C3)</f>
+        <v>2.0202020202020488E-3</v>
+      </c>
+      <c r="U3" s="13">
+        <f t="shared" ref="U3:U9" si="1">ABS((D3-L3)/D3)</f>
+        <v>1.6666666666666694E-2</v>
+      </c>
+      <c r="V3" s="13">
+        <f t="shared" ref="V3:V9" si="2">ABS((E3-M3)/E3)</f>
+        <v>6.5420560747663815E-3</v>
+      </c>
+      <c r="W3" s="13">
+        <f t="shared" ref="W3:W9" si="3">ABS((F3-N3)/F3)</f>
+        <v>5.4545454545454543E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -688,26 +767,52 @@
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="10">
-        <v>96.6</v>
-      </c>
-      <c r="K4" s="10">
-        <v>98.8</v>
-      </c>
-      <c r="L4" s="10">
-        <v>100.3</v>
-      </c>
-      <c r="M4" s="10">
-        <v>106.3</v>
-      </c>
-      <c r="N4" s="10">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="I4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="4">
+        <v>94.6</v>
+      </c>
+      <c r="K4" s="4">
+        <v>68.2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="M4" s="4">
+        <v>76.7</v>
+      </c>
+      <c r="N4" s="4">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="13">
+        <f t="shared" ref="S4:S9" si="4">ABS((B4-J4)/B4)</f>
+        <v>4.2105263157895334E-3</v>
+      </c>
+      <c r="T4" s="13">
+        <f t="shared" si="0"/>
+        <v>2.9411764705882769E-3</v>
+      </c>
+      <c r="U4" s="13">
+        <f t="shared" si="1"/>
+        <v>1.2500000000000079E-2</v>
+      </c>
+      <c r="V4" s="13">
+        <f t="shared" si="2"/>
+        <v>3.8961038961038592E-3</v>
+      </c>
+      <c r="W4" s="13">
+        <f t="shared" si="3"/>
+        <v>6.5384615384615305E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -729,16 +834,52 @@
       <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="1:14" ht="45.75" thickBot="1">
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="L5" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M5" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="13">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="T5" s="13">
+        <f t="shared" si="0"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="U5" s="13">
+        <f t="shared" si="1"/>
+        <v>0.30769230769230765</v>
+      </c>
+      <c r="V5" s="13">
+        <f t="shared" si="2"/>
+        <v>0.47500000000000009</v>
+      </c>
+      <c r="W5" s="13">
+        <f t="shared" si="3"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="21" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -760,26 +901,52 @@
       <c r="G6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="10">
-        <v>94.6</v>
-      </c>
-      <c r="K6" s="10">
-        <v>68.2</v>
-      </c>
-      <c r="L6" s="10">
-        <v>71.099999999999994</v>
-      </c>
-      <c r="M6" s="10">
-        <v>76.7</v>
-      </c>
-      <c r="N6" s="10">
-        <v>72.900000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="30.75" thickBot="1">
+      <c r="I6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.46</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1.46</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="13">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666689E-2</v>
+      </c>
+      <c r="U6" s="13">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428598E-2</v>
+      </c>
+      <c r="V6" s="13">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571494E-2</v>
+      </c>
+      <c r="W6" s="13">
+        <f t="shared" si="3"/>
+        <v>2.6666666666666689E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -801,16 +968,52 @@
       <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="1:14" ht="60.75" thickBot="1">
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="13">
+        <f>ABS((B7-(J7*1000))/B7)</f>
+        <v>4.6590141796083728E-2</v>
+      </c>
+      <c r="T7" s="13">
+        <f t="shared" ref="T7:W7" si="5">ABS((C7-(K7*1000))/C7)</f>
+        <v>4.6590141796083728E-2</v>
+      </c>
+      <c r="U7" s="13">
+        <f t="shared" si="5"/>
+        <v>4.061765693185633E-2</v>
+      </c>
+      <c r="V7" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5101772816808929E-2</v>
+      </c>
+      <c r="W7" s="13">
+        <f t="shared" si="5"/>
+        <v>0.17939168218497828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -832,26 +1035,52 @@
       <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="9">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K8" s="9">
-        <v>2.7</v>
-      </c>
-      <c r="L8" s="9">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M8" s="9">
-        <v>5.9</v>
-      </c>
-      <c r="N8" s="9">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="45.75" thickBot="1">
+      <c r="I8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="4">
+        <v>14.6</v>
+      </c>
+      <c r="K8" s="4">
+        <v>14.6</v>
+      </c>
+      <c r="L8" s="4">
+        <v>14.6</v>
+      </c>
+      <c r="M8" s="4">
+        <v>15.6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>23.7</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S8" s="13">
+        <f t="shared" si="4"/>
+        <v>0.14062499999999992</v>
+      </c>
+      <c r="T8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.14062499999999992</v>
+      </c>
+      <c r="U8" s="13">
+        <f t="shared" si="1"/>
+        <v>0.13178294573643404</v>
+      </c>
+      <c r="V8" s="13">
+        <f t="shared" si="2"/>
+        <v>0.13043478260869557</v>
+      </c>
+      <c r="W8" s="13">
+        <f t="shared" si="3"/>
+        <v>0.28108108108108104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="20.25" customHeight="1" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -873,160 +1102,155 @@
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.123</v>
+      </c>
+      <c r="K9" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="M9" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="T9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="U9" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="13">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="W9" s="13">
+        <f t="shared" si="3"/>
+        <v>0.77000000000000013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="K9" s="9">
-        <v>1.46</v>
-      </c>
-      <c r="L9" s="9">
-        <v>1.44</v>
-      </c>
-      <c r="M9" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="N9" s="9">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="30">
-      <c r="A10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="10">
-        <v>3.1</v>
-      </c>
-      <c r="K10" s="10">
-        <v>3.1</v>
-      </c>
-      <c r="L10" s="10">
-        <v>3.1</v>
-      </c>
-      <c r="M10" s="10">
-        <v>3</v>
-      </c>
-      <c r="N10" s="10">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
-      <c r="I11" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="I12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="10">
-        <v>14.6</v>
-      </c>
-      <c r="K12" s="10">
-        <v>14.6</v>
-      </c>
-      <c r="L12" s="10">
-        <v>14.6</v>
-      </c>
-      <c r="M12" s="10">
-        <v>15.6</v>
-      </c>
-      <c r="N12" s="10">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="I13" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:14" ht="45">
-      <c r="I14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="10">
-        <v>0.123</v>
-      </c>
-      <c r="K14" s="10">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M14" s="10">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="N14" s="10">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="30.75" thickBot="1">
-      <c r="I15" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="17" spans="9:16" ht="15.75">
-      <c r="I17" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
+      <c r="I17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
+  <mergeCells count="3">
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
   </mergeCells>
+  <conditionalFormatting sqref="S3:W9">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>